<commit_message>
Added MX-BBX and MX-DPBX accessories in panel accessories sheet for Austria, Italy, Slovakia, Netherlands and Denmark market
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_PanelAccessories_MX_Panels.xlsx
+++ b/Test Data/Gallery_PanelAccessories_MX_Panels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2DE9B-D377-4D57-843D-C773C4524659}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2B2ED6-98F5-4793-B1F1-3E452E6FAEAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="13" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Belgium" sheetId="14" r:id="rId1"/>
@@ -1272,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DCDDC4-460C-4F6D-BFDB-7441C6CDC348}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1949,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BC3B73-1EFC-4B72-9C36-EDADB60CCFB1}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>